<commit_message>
Download_file funcionando interfaz gráfica hasta descargas
</commit_message>
<xml_diff>
--- a/Download_file_Outlook/invoices_pdfs_downloads/correos_sin_adjuntos.xlsx
+++ b/Download_file_Outlook/invoices_pdfs_downloads/correos_sin_adjuntos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,32 +453,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-30 20:12:27+00:00</t>
+          <t>2025-09-24 12:03:39+00:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gab.rioja@gab.es</t>
+          <t>SAP España</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t>RE: 202540501668</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-09-24 12:03:39+00:00</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SAP España</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
         <is>
           <t>¡Únete a nosotros en el SAP Business Suite Innovation Day en Barcelona!</t>
         </is>

</xml_diff>